<commit_message>
Seed Generation updated to match new options
</commit_message>
<xml_diff>
--- a/SeedGeneration.xlsx
+++ b/SeedGeneration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PCSwitch\DocumentsX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SOTN Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E319C765-DC0B-470C-8DCD-49933BB482D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E1A3D8B-7D03-4BE2-BFB6-5ACD1D327032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{B6169CFC-9730-44E8-BEE8-6A502A3648CB}"/>
+    <workbookView xWindow="10920" yWindow="0" windowWidth="18225" windowHeight="15600" xr2:uid="{B6169CFC-9730-44E8-BEE8-6A502A3648CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="702">
   <si>
     <t>Mesatsu</t>
   </si>
@@ -1907,104 +1907,239 @@
     <t>fragtrap</t>
   </si>
   <si>
-    <t>Information About Magic Mirror / Looking Glass</t>
-  </si>
-  <si>
-    <t>Minimum Complexity 6 / 8</t>
-  </si>
-  <si>
-    <t>Spread Extension / Tourist Extension</t>
-  </si>
-  <si>
-    <t>Holy Glasses replaced by Magic Mirror</t>
-  </si>
-  <si>
-    <t>This teleport takes you to (roughly) the same point in the other castle</t>
-  </si>
-  <si>
-    <t>Many checks have been changed to add more complexity using this</t>
-  </si>
-  <si>
-    <t>Some new shortcuts added to improve routing in both castles</t>
-  </si>
-  <si>
     <t>Vanilla Item Sprites</t>
   </si>
   <si>
-    <t>Heart Vessel now also increases max MP and refills MP</t>
-  </si>
-  <si>
-    <t>Faster Teleporters</t>
-  </si>
-  <si>
-    <t>First Castle Entrance (NO3) has shortcut open to teleport to Outer Wall</t>
-  </si>
-  <si>
-    <t>This shortcut is closed in subsequent Castle Entrance visits (NP3)</t>
-  </si>
-  <si>
-    <t>Guaranteed shield / weapon drop from Leather Shield location in Alchemy Lab</t>
-  </si>
-  <si>
-    <t>This preset will result in players getting "out" of the castle. Save often.</t>
-  </si>
-  <si>
-    <t>Merman Statue check has escape requirements of Flight or Magic Mirror</t>
-  </si>
-  <si>
-    <t>Richter has the day off, Death does not</t>
-  </si>
-  <si>
-    <t>Axe Lord Armor provided in case the player gets hit outside of the castle</t>
-  </si>
-  <si>
-    <t>Cannot be used to skip bosses directly holding relics nor in castle center</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Magic Mirror let's you teleport between castles ( hold </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">✖ + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>▲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> )</t>
-    </r>
-  </si>
-  <si>
-    <t>Cannot be used while transformed (Bat, Wolf, Mist)</t>
-  </si>
-  <si>
     <t>glitch-two</t>
+  </si>
+  <si>
+    <t>lookingglass</t>
+  </si>
+  <si>
+    <t>casual</t>
+  </si>
+  <si>
+    <t>boss-rush</t>
+  </si>
+  <si>
+    <t>agonizetwtw</t>
+  </si>
+  <si>
+    <t>brawler</t>
+  </si>
+  <si>
+    <t>lobo</t>
+  </si>
+  <si>
+    <t>stensafe</t>
+  </si>
+  <si>
+    <t>gravis</t>
+  </si>
+  <si>
+    <t>Guarded Extension</t>
+  </si>
+  <si>
+    <t>Always $0 Shop Relic</t>
+  </si>
+  <si>
+    <t>Clock room statue always open</t>
+  </si>
+  <si>
+    <t>Magic Max Mode</t>
+  </si>
+  <si>
+    <t>Fast Warp Mode</t>
+  </si>
+  <si>
+    <t>Color Rando Mode</t>
+  </si>
+  <si>
+    <t>Unlocked Mode</t>
+  </si>
+  <si>
+    <t>Guaranteed Library Card at Resist thunder location</t>
+  </si>
+  <si>
+    <t>Guaranteed Weapon / Shield at Leather shield location</t>
+  </si>
+  <si>
+    <t>Guaranteed Bat in first castle</t>
+  </si>
+  <si>
+    <t>legolas</t>
+  </si>
+  <si>
+    <t>Information About Lucky Sevens</t>
+  </si>
+  <si>
+    <t>Minimum Complexity 7</t>
+  </si>
+  <si>
+    <t>Maximum Complexity 7</t>
+  </si>
+  <si>
+    <t>Warps for Deathwing's Lair and The Cave unlocked</t>
+  </si>
+  <si>
+    <t>Starting Stats are all 77, including HP, MP, and Hearts</t>
+  </si>
+  <si>
+    <t>Starting drop % chance is minimum 77%</t>
+  </si>
+  <si>
+    <t>Relics can be dropped by enemies, but will still be placed in their Guarded locations</t>
+  </si>
+  <si>
+    <t>Death is at the casino!</t>
+  </si>
+  <si>
+    <t>bingo</t>
+  </si>
+  <si>
+    <t>-t</t>
+  </si>
+  <si>
+    <t>-x</t>
+  </si>
+  <si>
+    <t>magic vessels</t>
+  </si>
+  <si>
+    <t>-z</t>
+  </si>
+  <si>
+    <t>-b</t>
+  </si>
+  <si>
+    <t>-l</t>
+  </si>
+  <si>
+    <t>anti-freeze</t>
+  </si>
+  <si>
+    <t>infinite wing smash</t>
+  </si>
+  <si>
+    <t>-R</t>
+  </si>
+  <si>
+    <t>no prologue</t>
+  </si>
+  <si>
+    <t>-E</t>
+  </si>
+  <si>
+    <t>enemy stat rando</t>
+  </si>
+  <si>
+    <t>-9</t>
+  </si>
+  <si>
+    <t>fast warps</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>-U</t>
+  </si>
+  <si>
+    <t>unlocked</t>
+  </si>
+  <si>
+    <t>-y</t>
+  </si>
+  <si>
+    <t>my purse</t>
+  </si>
+  <si>
+    <t>-S</t>
+  </si>
+  <si>
+    <t>surprise</t>
+  </si>
+  <si>
+    <t>first-castle</t>
+  </si>
+  <si>
+    <t>dog-life</t>
+  </si>
+  <si>
+    <t>cursed-night</t>
+  </si>
+  <si>
+    <t>skinwalker</t>
+  </si>
+  <si>
+    <t>glitchmaster</t>
+  </si>
+  <si>
+    <t>--sh</t>
+  </si>
+  <si>
+    <t>shop rando</t>
+  </si>
+  <si>
+    <t>sight-seer</t>
+  </si>
+  <si>
+    <t>mobility</t>
+  </si>
+  <si>
+    <t>safe</t>
+  </si>
+  <si>
+    <t>--ori</t>
+  </si>
+  <si>
+    <t>start rando</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>lucky-sevens</t>
+  </si>
+  <si>
+    <t>battle-mage</t>
+  </si>
+  <si>
+    <t>skill-expression</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2019,25 +2154,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2080,9 +2196,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2098,6 +2214,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>333226</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>189713</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3497BF0-E81A-2E0A-9767-1D3B8FEB3F53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14211300" y="180975"/>
+          <a:ext cx="1190476" cy="6295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2397,10 +2562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2114AA48-3BFF-4EB5-A065-BA74F06B192B}">
-  <dimension ref="A1:M100"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2410,7 +2575,7 @@
     <col min="7" max="7" width="3" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" customWidth="1"/>
     <col min="11" max="11" width="23.85546875" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
     <col min="13" max="13" width="102.28515625" bestFit="1" customWidth="1"/>
@@ -2419,27 +2584,27 @@
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <f ca="1">NOW()</f>
-        <v>45442.050972106481</v>
+        <v>45655.830477546297</v>
       </c>
       <c r="B1" s="2">
-        <f t="shared" ref="B1:B3" ca="1" si="0">RIGHT(A1,2)*ROW()*RANDBETWEEN(1,3)</f>
-        <v>65</v>
+        <f ca="1">RIGHT(A1,2)*ROW()*RANDBETWEEN(1,3)</f>
+        <v>189</v>
       </c>
       <c r="C1">
         <f ca="1">ROUND(((B1*11)/7),2)</f>
-        <v>102.14</v>
+        <v>297</v>
       </c>
       <c r="D1" t="str">
         <f ca="1">TEXT(C1,"0000.00")</f>
-        <v>0102.14</v>
+        <v>0297.00</v>
       </c>
       <c r="E1" t="str">
-        <f t="shared" ref="E1:E3" ca="1" si="1">MID(D1,3,2)</f>
-        <v>02</v>
+        <f ca="1">MID(D1,3,2)</f>
+        <v>97</v>
       </c>
       <c r="F1">
         <f ca="1">VALUE(E1)</f>
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H1" t="s">
         <v>82</v>
@@ -2453,28 +2618,28 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <f t="shared" ref="A2:A3" ca="1" si="2">NOW()</f>
-        <v>45442.050972106481</v>
+        <f ca="1">NOW()</f>
+        <v>45655.830477546297</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>260</v>
+        <f ca="1">RIGHT(A2,2)*ROW()*RANDBETWEEN(1,3)</f>
+        <v>378</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C3" ca="1" si="3">ROUND(((B2*11)/7),2)</f>
-        <v>408.57</v>
+        <f ca="1">ROUND(((B2*11)/7),2)</f>
+        <v>594</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D3" ca="1" si="4">TEXT(C2,"0000.00")</f>
-        <v>0408.57</v>
+        <f ca="1">TEXT(C2,"0000.00")</f>
+        <v>0594.00</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>08</v>
+        <f ca="1">MID(D2,3,2)</f>
+        <v>94</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F3" ca="1" si="5">VALUE(E2)</f>
-        <v>8</v>
+        <f ca="1">VALUE(E2)</f>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -2484,37 +2649,37 @@
       </c>
       <c r="K2" t="str">
         <f ca="1">INDEX($H$1:$H$100,F1)&amp;INDEX($I$1:$I$100,F2)&amp;F3</f>
-        <v>MesatsuZombie12</v>
+        <v>BucolicSurge94</v>
       </c>
       <c r="M2" t="str">
         <f ca="1">"node randomize -t -p "&amp;K4 &amp; " -s "&amp;K2 &amp; " -o .\seeds\"&amp;PROPER(K4)&amp;"-"&amp;K2&amp;".ppf"</f>
-        <v>node randomize -t -p crash-course -s MesatsuZombie12 -o .\seeds\Crash-Course-MesatsuZombie12.ppf</v>
+        <v>node randomize -t -p battle-mage -s BucolicSurge94 -o .\seeds\Battle-Mage-BucolicSurge94.ppf</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>45442.050972106481</v>
+        <f ca="1">NOW()</f>
+        <v>45655.830477546297</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>390</v>
+        <f ca="1">RIGHT(A3,2)*ROW()*RANDBETWEEN(1,3)</f>
+        <v>378</v>
       </c>
       <c r="C3">
-        <f t="shared" ca="1" si="3"/>
-        <v>612.86</v>
+        <f ca="1">ROUND(((B3*11)/7),2)</f>
+        <v>594</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>0612.86</v>
+        <f ca="1">TEXT(C3,"0000.00")</f>
+        <v>0594.00</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <f ca="1">MID(D3,3,2)</f>
+        <v>94</v>
       </c>
       <c r="F3">
-        <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <f ca="1">VALUE(E3)</f>
+        <v>94</v>
       </c>
       <c r="H3" t="s">
         <v>1</v>
@@ -2527,6 +2692,30 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f ca="1">NOW()</f>
+        <v>45655.830477546297</v>
+      </c>
+      <c r="B4" s="2">
+        <f ca="1">RIGHT(A4,2)*ROW()*RANDBETWEEN(1,3)</f>
+        <v>504</v>
+      </c>
+      <c r="C4">
+        <f ca="1">ROUND(((B4*11)/7),2)</f>
+        <v>792</v>
+      </c>
+      <c r="D4" t="str">
+        <f ca="1">TEXT(C4,"0000.00")</f>
+        <v>0792.00</v>
+      </c>
+      <c r="E4" t="str">
+        <f ca="1">MID(D4,3,2)</f>
+        <v>92</v>
+      </c>
+      <c r="F4">
+        <f ca="1">VALUE(E4)</f>
+        <v>92</v>
+      </c>
       <c r="H4" t="s">
         <v>2</v>
       </c>
@@ -2534,11 +2723,11 @@
         <v>81</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>211</v>
+        <v>691</v>
       </c>
       <c r="M4" t="str">
         <f ca="1">SUBSTITUTE(M2," -t "," -t --opt ~m ")</f>
-        <v>node randomize -t --opt ~m -p crash-course -s MesatsuZombie12 -o .\seeds\Crash-Course-MesatsuZombie12.ppf</v>
+        <v>node randomize -t --opt ~m -p battle-mage -s BucolicSurge94 -o .\seeds\Battle-Mage-BucolicSurge94.ppf</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2556,6 +2745,10 @@
       <c r="I6" t="s">
         <v>85</v>
       </c>
+      <c r="M6" t="str">
+        <f ca="1">SUBSTITUTE(M2," -t "," ")</f>
+        <v>node randomize -p battle-mage -s BucolicSurge94 -o .\seeds\Battle-Mage-BucolicSurge94.ppf</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
@@ -2573,6 +2766,10 @@
         <v>87</v>
       </c>
       <c r="K8" s="4"/>
+      <c r="M8" t="str">
+        <f ca="1">SUBSTITUTE(M2,"-t -p","-t -z -9 -b -x -E -p")</f>
+        <v>node randomize -t -z -9 -b -x -E -p battle-mage -s BucolicSurge94 -o .\seeds\Battle-Mage-BucolicSurge94.ppf</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
@@ -2591,11 +2788,18 @@
       </c>
       <c r="K10" s="4"/>
       <c r="M10" t="str">
-        <f>M6&amp;" -vvvv"</f>
-        <v xml:space="preserve"> -vvvv</v>
+        <f ca="1">M6&amp;" -vvvv"</f>
+        <v>node randomize -p battle-mage -s BucolicSurge94 -o .\seeds\Battle-Mage-BucolicSurge94.ppf -vvvv</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E11" t="str">
+        <f ca="1">INDEX(F11:F20,ROUND(F4/10,0))</f>
+        <v>i</v>
+      </c>
+      <c r="F11" t="s">
+        <v>693</v>
+      </c>
       <c r="H11" t="s">
         <v>181</v>
       </c>
@@ -2604,6 +2808,9 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>694</v>
+      </c>
       <c r="H12" t="s">
         <v>182</v>
       </c>
@@ -2612,10 +2819,13 @@
       </c>
       <c r="M12" t="str">
         <f ca="1">SUBSTITUTE(M2," -t "," -t --opt r:x:tourist ")</f>
-        <v>node randomize -t --opt r:x:tourist -p crash-course -s MesatsuZombie12 -o .\seeds\Crash-Course-MesatsuZombie12.ppf</v>
+        <v>node randomize -t --opt r:x:tourist -p battle-mage -s BucolicSurge94 -o .\seeds\Battle-Mage-BucolicSurge94.ppf</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>695</v>
+      </c>
       <c r="H13" t="s">
         <v>183</v>
       </c>
@@ -2624,14 +2834,24 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>696</v>
+      </c>
       <c r="H14" t="s">
         <v>7</v>
       </c>
       <c r="I14" t="s">
         <v>92</v>
       </c>
+      <c r="M14" t="str">
+        <f ca="1">SUBSTITUTE(M8," -p"," -"&amp;J16&amp;" -p")</f>
+        <v>node randomize -t -z -9 -b -x -E --m i -p battle-mage -s BucolicSurge94 -o .\seeds\Battle-Mage-BucolicSurge94.ppf</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>697</v>
+      </c>
       <c r="H15" t="s">
         <v>8</v>
       </c>
@@ -2640,163 +2860,254 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>699</v>
+      </c>
       <c r="H16" t="s">
         <v>9</v>
       </c>
       <c r="I16" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="17" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="5" t="str">
+        <f ca="1">IF(E11=0," ","-m "&amp;E11)</f>
+        <v>-m i</v>
+      </c>
+      <c r="L16" t="s">
+        <v>670</v>
+      </c>
+      <c r="M16" t="str">
+        <f ca="1">TRIM("node randomize "&amp;$K$47&amp;" -p "&amp;$K$4&amp;" -s "&amp;$K$2&amp;" -o .\seeds\"&amp;PROPER($K$4)&amp;"-"&amp;$K$2&amp;".ppf")</f>
+        <v>node randomize -t -z --sh -m i -p battle-mage -s BucolicSurge94 -o .\seeds\Battle-Mage-BucolicSurge94.ppf</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>700</v>
+      </c>
       <c r="H17" t="s">
         <v>10</v>
       </c>
       <c r="I17" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="K17" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="L17" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>701</v>
+      </c>
       <c r="H18" t="s">
         <v>11</v>
       </c>
       <c r="I18" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="K18" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="19" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>698</v>
+      </c>
       <c r="H19" t="s">
         <v>12</v>
       </c>
       <c r="I19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="K19" t="s">
+        <v>662</v>
+      </c>
+      <c r="L19" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>0</v>
+      </c>
       <c r="H20" t="s">
         <v>13</v>
       </c>
       <c r="I20" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="K20" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="21" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
         <v>14</v>
       </c>
       <c r="I21" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="22" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="K21" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="22" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>15</v>
       </c>
       <c r="I22" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="K22" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="23" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>16</v>
       </c>
       <c r="I23" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="24" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="K23" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="24" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>17</v>
       </c>
       <c r="I24" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="K24" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>18</v>
       </c>
       <c r="I25" t="s">
         <v>103</v>
       </c>
+      <c r="J25" s="5" t="s">
+        <v>671</v>
+      </c>
       <c r="K25" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="26" spans="8:11" x14ac:dyDescent="0.25">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="26" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>19</v>
       </c>
       <c r="I26" t="s">
         <v>104</v>
       </c>
+      <c r="J26" s="5" t="s">
+        <v>673</v>
+      </c>
       <c r="K26" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="27" spans="8:11" x14ac:dyDescent="0.25">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="27" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>20</v>
       </c>
       <c r="I27" t="s">
         <v>105</v>
       </c>
+      <c r="J27" s="5" t="s">
+        <v>675</v>
+      </c>
       <c r="K27" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="28" spans="8:11" x14ac:dyDescent="0.25">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="28" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>21</v>
       </c>
       <c r="I28" t="s">
         <v>106</v>
       </c>
+      <c r="J28" s="5" t="s">
+        <v>682</v>
+      </c>
       <c r="K28" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="8:11" x14ac:dyDescent="0.25">
+        <v>683</v>
+      </c>
+      <c r="L28" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="29" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
         <v>22</v>
       </c>
       <c r="I29" t="s">
         <v>107</v>
       </c>
+      <c r="J29" s="5" t="s">
+        <v>687</v>
+      </c>
       <c r="K29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="8:11" x14ac:dyDescent="0.25">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="30" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>23</v>
       </c>
       <c r="I30" t="s">
         <v>108</v>
       </c>
-      <c r="K30" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="8:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>24</v>
       </c>
       <c r="I31" t="s">
         <v>99</v>
       </c>
-      <c r="K31" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="8:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
         <v>25</v>
       </c>
       <c r="I32" t="s">
         <v>112</v>
-      </c>
-      <c r="K32" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="33" spans="8:11" x14ac:dyDescent="0.25">
@@ -2806,8 +3117,9 @@
       <c r="I33" t="s">
         <v>113</v>
       </c>
-      <c r="K33" t="s">
-        <v>208</v>
+      <c r="J33" t="str">
+        <f>J17</f>
+        <v>-t</v>
       </c>
     </row>
     <row r="34" spans="8:11" x14ac:dyDescent="0.25">
@@ -2817,8 +3129,13 @@
       <c r="I34" t="s">
         <v>114</v>
       </c>
-      <c r="K34" t="s">
-        <v>209</v>
+      <c r="J34" t="str">
+        <f>IF(ISBLANK($L18),"",J18)</f>
+        <v/>
+      </c>
+      <c r="K34" t="str">
+        <f>IF(ISBLANK($L18),"",K18)</f>
+        <v/>
       </c>
     </row>
     <row r="35" spans="8:11" x14ac:dyDescent="0.25">
@@ -2828,8 +3145,13 @@
       <c r="I35" t="s">
         <v>115</v>
       </c>
-      <c r="K35" t="s">
-        <v>210</v>
+      <c r="J35" t="str">
+        <f t="shared" ref="J35:J45" si="0">IF(ISBLANK($L19),"",J19)</f>
+        <v>-z</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" ref="K35:K44" si="1">IF(ISBLANK(L19),"",K19)</f>
+        <v>anti-freeze</v>
       </c>
     </row>
     <row r="36" spans="8:11" x14ac:dyDescent="0.25">
@@ -2839,8 +3161,13 @@
       <c r="I36" t="s">
         <v>116</v>
       </c>
-      <c r="K36" t="s">
-        <v>211</v>
+      <c r="J36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="37" spans="8:11" x14ac:dyDescent="0.25">
@@ -2850,8 +3177,13 @@
       <c r="I37" t="s">
         <v>117</v>
       </c>
-      <c r="K37" t="s">
-        <v>212</v>
+      <c r="J37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="38" spans="8:11" x14ac:dyDescent="0.25">
@@ -2861,8 +3193,13 @@
       <c r="I38" t="s">
         <v>118</v>
       </c>
-      <c r="K38" t="s">
-        <v>213</v>
+      <c r="J38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="39" spans="8:11" x14ac:dyDescent="0.25">
@@ -2872,8 +3209,13 @@
       <c r="I39" t="s">
         <v>119</v>
       </c>
-      <c r="K39" t="s">
-        <v>214</v>
+      <c r="J39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="40" spans="8:11" x14ac:dyDescent="0.25">
@@ -2883,8 +3225,13 @@
       <c r="I40" t="s">
         <v>120</v>
       </c>
-      <c r="K40" t="s">
-        <v>215</v>
+      <c r="J40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="41" spans="8:11" x14ac:dyDescent="0.25">
@@ -2894,8 +3241,13 @@
       <c r="I41" t="s">
         <v>121</v>
       </c>
-      <c r="K41" t="s">
-        <v>216</v>
+      <c r="J41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="42" spans="8:11" x14ac:dyDescent="0.25">
@@ -2905,8 +3257,13 @@
       <c r="I42" t="s">
         <v>122</v>
       </c>
-      <c r="K42" t="s">
-        <v>217</v>
+      <c r="J42" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="43" spans="8:11" x14ac:dyDescent="0.25">
@@ -2916,8 +3273,13 @@
       <c r="I43" t="s">
         <v>123</v>
       </c>
-      <c r="K43" t="s">
-        <v>218</v>
+      <c r="J43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="44" spans="8:11" x14ac:dyDescent="0.25">
@@ -2927,8 +3289,13 @@
       <c r="I44" t="s">
         <v>124</v>
       </c>
-      <c r="K44" t="s">
-        <v>620</v>
+      <c r="J44" t="str">
+        <f t="shared" si="0"/>
+        <v>--sh</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="1"/>
+        <v>shop rando</v>
       </c>
     </row>
     <row r="45" spans="8:11" x14ac:dyDescent="0.25">
@@ -2938,8 +3305,13 @@
       <c r="I45" t="s">
         <v>125</v>
       </c>
-      <c r="K45" t="s">
-        <v>621</v>
+      <c r="J45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" ref="K45" si="2">IF(ISBLANK(L29),"",K29)</f>
+        <v/>
       </c>
     </row>
     <row r="46" spans="8:11" x14ac:dyDescent="0.25">
@@ -2949,9 +3321,6 @@
       <c r="I46" t="s">
         <v>126</v>
       </c>
-      <c r="K46" t="s">
-        <v>622</v>
-      </c>
     </row>
     <row r="47" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H47" t="s">
@@ -2960,8 +3329,13 @@
       <c r="I47" t="s">
         <v>127</v>
       </c>
-      <c r="K47" t="s">
-        <v>623</v>
+      <c r="J47" t="str">
+        <f ca="1">J16</f>
+        <v>-m i</v>
+      </c>
+      <c r="K47" t="str">
+        <f ca="1">_xlfn.TEXTJOIN(" ",TRUE,J33:J47)</f>
+        <v>-t -z --sh -m i</v>
       </c>
     </row>
     <row r="48" spans="8:11" x14ac:dyDescent="0.25">
@@ -2971,8 +3345,9 @@
       <c r="I48" t="s">
         <v>128</v>
       </c>
-      <c r="K48" t="s">
-        <v>624</v>
+      <c r="K48" t="str">
+        <f>_xlfn.TEXTJOIN(", ",TRUE,K34:K46)</f>
+        <v>anti-freeze, shop rando</v>
       </c>
     </row>
     <row r="49" spans="8:11" x14ac:dyDescent="0.25">
@@ -2982,9 +3357,6 @@
       <c r="I49" t="s">
         <v>129</v>
       </c>
-      <c r="K49" t="s">
-        <v>625</v>
-      </c>
     </row>
     <row r="50" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H50" t="s">
@@ -2993,9 +3365,6 @@
       <c r="I50" t="s">
         <v>130</v>
       </c>
-      <c r="K50" t="s">
-        <v>646</v>
-      </c>
     </row>
     <row r="51" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H51" t="s">
@@ -3028,6 +3397,9 @@
       <c r="I54" t="s">
         <v>134</v>
       </c>
+      <c r="K54" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="55" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H55" t="s">
@@ -3036,6 +3408,9 @@
       <c r="I55" t="s">
         <v>135</v>
       </c>
+      <c r="K55" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="56" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H56" t="s">
@@ -3044,6 +3419,9 @@
       <c r="I56" t="s">
         <v>136</v>
       </c>
+      <c r="K56" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="57" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H57" t="s">
@@ -3052,6 +3430,9 @@
       <c r="I57" t="s">
         <v>137</v>
       </c>
+      <c r="K57" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="58" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H58" t="s">
@@ -3060,6 +3441,9 @@
       <c r="I58" t="s">
         <v>138</v>
       </c>
+      <c r="K58" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="59" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H59" t="s">
@@ -3068,6 +3452,9 @@
       <c r="I59" t="s">
         <v>139</v>
       </c>
+      <c r="K59" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="60" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H60" t="s">
@@ -3076,6 +3463,9 @@
       <c r="I60" t="s">
         <v>140</v>
       </c>
+      <c r="K60" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="61" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H61" t="s">
@@ -3084,6 +3474,9 @@
       <c r="I61" t="s">
         <v>141</v>
       </c>
+      <c r="K61" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="62" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H62" t="s">
@@ -3092,6 +3485,9 @@
       <c r="I62" t="s">
         <v>142</v>
       </c>
+      <c r="K62" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="63" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H63" t="s">
@@ -3100,6 +3496,9 @@
       <c r="I63" t="s">
         <v>143</v>
       </c>
+      <c r="K63" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="64" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H64" t="s">
@@ -3108,299 +3507,420 @@
       <c r="I64" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K64" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="65" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H65" t="s">
         <v>155</v>
       </c>
       <c r="I65" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K65" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="66" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H66" t="s">
         <v>156</v>
       </c>
       <c r="I66" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K66" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H67" t="s">
         <v>157</v>
       </c>
       <c r="I67" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K67" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="68" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H68" t="s">
         <v>158</v>
       </c>
       <c r="I68" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K68" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="69" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H69" t="s">
         <v>159</v>
       </c>
       <c r="I69" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K69" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="70" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H70" t="s">
         <v>160</v>
       </c>
       <c r="I70" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K70" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H71" t="s">
         <v>55</v>
       </c>
       <c r="I71" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K71" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="72" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H72" t="s">
         <v>56</v>
       </c>
       <c r="I72" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K72" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H73" t="s">
         <v>57</v>
       </c>
       <c r="I73" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K73" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="74" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H74" t="s">
         <v>58</v>
       </c>
       <c r="I74" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K74" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="75" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H75" t="s">
         <v>6</v>
       </c>
       <c r="I75" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K75" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="76" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H76" t="s">
         <v>168</v>
       </c>
       <c r="I76" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K76" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="77" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H77" t="s">
         <v>169</v>
       </c>
       <c r="I77" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K77" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="78" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H78" t="s">
         <v>111</v>
       </c>
       <c r="I78" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K78" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="79" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H79" t="s">
         <v>110</v>
       </c>
       <c r="I79" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K79" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="80" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H80" t="s">
         <v>59</v>
       </c>
       <c r="I80" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K80" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="81" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H81" t="s">
         <v>60</v>
       </c>
       <c r="I81" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K81" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="82" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H82" t="s">
         <v>61</v>
       </c>
       <c r="I82" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K82" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="83" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H83" t="s">
         <v>62</v>
       </c>
       <c r="I83" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K83" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="84" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H84" t="s">
         <v>63</v>
       </c>
       <c r="I84" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K84" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="85" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H85" t="s">
         <v>64</v>
       </c>
       <c r="I85" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K85" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="86" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H86" t="s">
         <v>65</v>
       </c>
       <c r="I86" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K86" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="87" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H87" t="s">
         <v>66</v>
       </c>
       <c r="I87" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K87" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="88" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H88" t="s">
         <v>67</v>
       </c>
       <c r="I88" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K88" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="89" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H89" t="s">
         <v>68</v>
       </c>
       <c r="I89" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K89" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="90" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H90" t="s">
         <v>69</v>
       </c>
       <c r="I90" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K90" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="91" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H91" t="s">
         <v>70</v>
       </c>
       <c r="I91" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K91" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="92" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H92" t="s">
         <v>71</v>
       </c>
       <c r="I92" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K92" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="93" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H93" t="s">
         <v>72</v>
       </c>
       <c r="I93" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K93" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="94" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H94" t="s">
         <v>73</v>
       </c>
       <c r="I94" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K94" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="95" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H95" t="s">
         <v>74</v>
       </c>
       <c r="I95" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K95" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="96" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H96" t="s">
         <v>75</v>
       </c>
       <c r="I96" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K96" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="97" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H97" t="s">
         <v>76</v>
       </c>
       <c r="I97" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K97" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="98" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H98" t="s">
         <v>77</v>
       </c>
       <c r="I98" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K98" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="99" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H99" t="s">
         <v>78</v>
       </c>
       <c r="I99" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="K99" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="100" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H100" t="s">
         <v>94</v>
       </c>
       <c r="I100" t="s">
         <v>196</v>
+      </c>
+      <c r="K100" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="101" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K101" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="102" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K102" t="s">
+        <v>692</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4" xr:uid="{52954BD4-7E9F-43F1-ABD7-1B3E1CB07824}">
-      <formula1>$K$25:$K$50</formula1>
+      <formula1>$K$54:$K$129</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6 K10" xr:uid="{6C4EC44C-E667-4A90-976F-C1E937B06FBC}">
       <formula1>#REF!</formula1>
@@ -3418,7 +3938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB6F30C-EB11-4DFE-9834-DFB7693A55FB}">
   <dimension ref="A1:A401"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -5436,149 +5956,165 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBD0B89-74A9-432C-9D08-5B3021CE010F}">
-  <dimension ref="B3:C22"/>
+  <dimension ref="B3:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C22"/>
+      <selection activeCell="B3" sqref="B3:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="3.140625" customWidth="1"/>
-    <col min="3" max="3" width="67.42578125" customWidth="1"/>
+    <col min="3" max="3" width="72.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
+        <v>647</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>626</v>
       </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>627</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>628</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>633</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>629</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>639</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>632</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>634</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>635</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>636</v>
-      </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>637</v>
-      </c>
+      <c r="B17" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>638</v>
-      </c>
-      <c r="C18" s="5"/>
+      <c r="B18" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>640</v>
-      </c>
-      <c r="C19" s="5"/>
+      <c r="B19" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="C20" s="5"/>
+      <c r="B20" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="C20" s="6"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="C21" s="5"/>
+      <c r="B21" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
-        <v>639</v>
-      </c>
-      <c r="C22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
+  <mergeCells count="21">
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>